<commit_message>
Adaugare problema arhitectura noua
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrei/Downloads/CheckLists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrei/Documents/Facultate/Anul 3/Semestrul 2/VVSS/Pizza/Docs/Lab01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEEA5FA-CC45-7E4E-8DBF-01B8C7C89017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D4BB40-D1A5-AE4C-A79D-0A919EE91983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -182,12 +182,6 @@
     <t>1 ora</t>
   </si>
   <si>
-    <t>Lipsesc pachetele din diagrama</t>
-  </si>
-  <si>
-    <t>A02</t>
-  </si>
-  <si>
     <t>Class Diagram</t>
   </si>
   <si>
@@ -201,6 +195,36 @@
   </si>
   <si>
     <t>A01</t>
+  </si>
+  <si>
+    <t>KitchenGUIController - 53</t>
+  </si>
+  <si>
+    <t>Nu este verificat daca exista elemente selectate pentru a le putea da cook.</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>Inainte de a da ready la o comanda, ar trebui verificat ca este si selectata o comanda, altfel va pusca programul.</t>
+  </si>
+  <si>
+    <t>KitchenGUIController - 62</t>
+  </si>
+  <si>
+    <t>Cand se alege cantitatea unui produs nu ar trebui sa poti alege si 0 (nu are sens sa adaugi la comanda "nimic")</t>
+  </si>
+  <si>
+    <t>OrdersGUIController - 131</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>2 ore</t>
+  </si>
+  <si>
+    <t>Nu ar trebui date fisierele de input ca parametru la repository, o solutie mai buna ar fi crearea unui fisier de configurari de unde sa fie extrase</t>
   </si>
 </sst>
 </file>
@@ -415,6 +439,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -456,10 +484,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,8 +624,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>100337</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19057</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -990,19 +1014,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1015,7 +1039,7 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="17">
@@ -1026,14 +1050,14 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="26"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="21" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -1044,14 +1068,14 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="28"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="21" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="3">
@@ -1063,19 +1087,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="21"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="22">
         <v>45005</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
@@ -1283,8 +1307,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1303,19 +1327,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1328,7 +1352,7 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="17">
@@ -1339,14 +1363,14 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="21" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -1357,14 +1381,14 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="21" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="3">
@@ -1376,19 +1400,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="21"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="22">
         <v>45005</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
@@ -1404,18 +1428,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1424,13 +1448,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -1439,13 +1463,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1605,8 +1629,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1626,19 +1650,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1651,7 +1675,7 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="17">
@@ -1662,14 +1686,14 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="21" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -1680,14 +1704,14 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="21" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="3">
@@ -1699,19 +1723,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="21"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="22">
         <v>45005</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
@@ -1727,31 +1751,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
@@ -1920,7 +1962,9 @@
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1966,19 +2010,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1998,8 +2042,8 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -2010,8 +2054,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2023,8 +2067,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -2254,11 +2298,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>